<commit_message>
Bildung_WikiFernlernen.csv - manual update data/wiki_200615.xlsx - new base data prepareWIKI.R - changes in loadSingleFile(), select Hits instead of Visits README.md, data/wiki_meta.json - minor changes
</commit_message>
<xml_diff>
--- a/data/wiki_200508.xlsx
+++ b/data/wiki_200508.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/schulinformatik/Desktop/Statistik Wiki/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\B251PFI\Documents\Rworkspace\2020_covid19_edu_vsa\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{47B39BE3-CCCC-4C49-9787-5333053F9DFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28680" windowHeight="19520" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28680" windowHeight="19515" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Export-Zusammenfassung" sheetId="1" r:id="rId1"/>
@@ -89,7 +88,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0#%"/>
   </numFmts>
@@ -1606,25 +1605,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:D16"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="13" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="12.95" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
-    <col min="2" max="4" width="33.6640625" customWidth="1"/>
+    <col min="2" max="4" width="33.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" ht="50" customHeight="1">
+    <row r="3" spans="2:4" ht="50.1" customHeight="1">
       <c r="B3" s="29" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
     </row>
-    <row r="7" spans="2:4" ht="19">
+    <row r="7" spans="2:4" ht="36">
       <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
@@ -1635,14 +1634,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="17">
+    <row r="9" spans="2:4" ht="15">
       <c r="B9" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="2:4" ht="17">
+    <row r="10" spans="2:4" ht="15">
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
         <v>5</v>
@@ -1651,14 +1650,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="17">
+    <row r="11" spans="2:4" ht="15">
       <c r="B11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="2:4" ht="17">
+    <row r="12" spans="2:4" ht="15">
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
         <v>5</v>
@@ -1667,14 +1666,14 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="17">
+    <row r="13" spans="2:4" ht="15">
       <c r="B13" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="2:4" ht="17">
+    <row r="14" spans="2:4" ht="15">
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
         <v>5</v>
@@ -1683,14 +1682,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="17">
+    <row r="15" spans="2:4" ht="15">
       <c r="B15" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="2:4" ht="17">
+    <row r="16" spans="2:4" ht="15">
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
         <v>5</v>
@@ -1704,17 +1703,17 @@
     <mergeCell ref="B3:D3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D10" location="'Februar 2020'!R2C1" display="Februar 2020" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D12" location="'Januar 2020'!R2C1" display="Januar 2020" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D14" location="'März 2020'!R2C1" display="März 2020" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="D16" location="'April 2020'!R2C1" display="April 2020" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D10" location="'Februar 2020'!R2C1" display="Februar 2020"/>
+    <hyperlink ref="D12" location="'Januar 2020'!R2C1" display="Januar 2020"/>
+    <hyperlink ref="D14" location="'März 2020'!R2C1" display="März 2020"/>
+    <hyperlink ref="D16" location="'April 2020'!R2C1" display="April 2020"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -1724,10 +1723,10 @@
       <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.28515625" defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
-    <col min="1" max="14" width="16.33203125" style="5" customWidth="1"/>
-    <col min="15" max="16384" width="16.33203125" style="5"/>
+    <col min="1" max="14" width="16.28515625" style="5" customWidth="1"/>
+    <col min="15" max="16384" width="16.28515625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="27.75" customHeight="1">
@@ -1777,7 +1776,7 @@
       <c r="L3" s="9"/>
       <c r="M3" s="9"/>
     </row>
-    <row r="4" spans="1:13" ht="78.25" customHeight="1">
+    <row r="4" spans="1:13" ht="78.2" customHeight="1">
       <c r="A4" s="10" t="s">
         <v>6</v>
       </c>
@@ -1794,7 +1793,7 @@
       <c r="L4" s="12"/>
       <c r="M4" s="12"/>
     </row>
-    <row r="5" spans="1:13" ht="20" customHeight="1">
+    <row r="5" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A5" s="13"/>
       <c r="B5" s="11"/>
       <c r="C5" s="12"/>
@@ -1809,7 +1808,7 @@
       <c r="L5" s="12"/>
       <c r="M5" s="12"/>
     </row>
-    <row r="6" spans="1:13" ht="18.25" customHeight="1">
+    <row r="6" spans="1:13" ht="18.2" customHeight="1">
       <c r="A6" s="14" t="s">
         <v>7</v>
       </c>
@@ -1838,7 +1837,7 @@
       </c>
       <c r="M6" s="33"/>
     </row>
-    <row r="7" spans="1:13" ht="20" customHeight="1">
+    <row r="7" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A7" s="13"/>
       <c r="B7" s="11"/>
       <c r="C7" s="12"/>
@@ -1853,7 +1852,7 @@
       <c r="L7" s="12"/>
       <c r="M7" s="12"/>
     </row>
-    <row r="8" spans="1:13" ht="18.25" customHeight="1">
+    <row r="8" spans="1:13" ht="18.2" customHeight="1">
       <c r="A8" s="15">
         <v>1</v>
       </c>
@@ -1894,7 +1893,7 @@
         <v>1.7100000000000001E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="18.25" customHeight="1">
+    <row r="9" spans="1:13" ht="18.2" customHeight="1">
       <c r="A9" s="15">
         <v>2</v>
       </c>
@@ -1935,7 +1934,7 @@
         <v>2.6700000000000002E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="18.25" customHeight="1">
+    <row r="10" spans="1:13" ht="18.2" customHeight="1">
       <c r="A10" s="20">
         <v>3</v>
       </c>
@@ -1976,7 +1975,7 @@
         <v>3.4299999999999997E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="18.25" customHeight="1">
+    <row r="11" spans="1:13" ht="18.2" customHeight="1">
       <c r="A11" s="20">
         <v>4</v>
       </c>
@@ -2017,7 +2016,7 @@
         <v>3.8199999999999998E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="18.25" customHeight="1">
+    <row r="12" spans="1:13" ht="18.2" customHeight="1">
       <c r="A12" s="20">
         <v>5</v>
       </c>
@@ -2058,7 +2057,7 @@
         <v>5.57E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="18.25" customHeight="1">
+    <row r="13" spans="1:13" ht="18.2" customHeight="1">
       <c r="A13" s="20">
         <v>6</v>
       </c>
@@ -2099,7 +2098,7 @@
         <v>4.1099999999999998E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="18.25" customHeight="1">
+    <row r="14" spans="1:13" ht="18.2" customHeight="1">
       <c r="A14" s="20">
         <v>7</v>
       </c>
@@ -2140,7 +2139,7 @@
         <v>3.1099999999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="18.25" customHeight="1">
+    <row r="15" spans="1:13" ht="18.2" customHeight="1">
       <c r="A15" s="15">
         <v>8</v>
       </c>
@@ -2181,7 +2180,7 @@
         <v>3.78E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="18.25" customHeight="1">
+    <row r="16" spans="1:13" ht="18.2" customHeight="1">
       <c r="A16" s="15">
         <v>9</v>
       </c>
@@ -2222,7 +2221,7 @@
         <v>3.6299999999999999E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="18.25" customHeight="1">
+    <row r="17" spans="1:13" ht="18.2" customHeight="1">
       <c r="A17" s="20">
         <v>10</v>
       </c>
@@ -2263,7 +2262,7 @@
         <v>3.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="18.25" customHeight="1">
+    <row r="18" spans="1:13" ht="18.2" customHeight="1">
       <c r="A18" s="20">
         <v>11</v>
       </c>
@@ -2304,7 +2303,7 @@
         <v>5.7500000000000002E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="18.25" customHeight="1">
+    <row r="19" spans="1:13" ht="18.2" customHeight="1">
       <c r="A19" s="20">
         <v>12</v>
       </c>
@@ -2345,7 +2344,7 @@
         <v>3.9699999999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="18.25" customHeight="1">
+    <row r="20" spans="1:13" ht="18.2" customHeight="1">
       <c r="A20" s="20">
         <v>13</v>
       </c>
@@ -2386,7 +2385,7 @@
         <v>3.1399999999999997E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="18.25" customHeight="1">
+    <row r="21" spans="1:13" ht="18.2" customHeight="1">
       <c r="A21" s="20">
         <v>14</v>
       </c>
@@ -2427,7 +2426,7 @@
         <v>2.76E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="18.25" customHeight="1">
+    <row r="22" spans="1:13" ht="18.2" customHeight="1">
       <c r="A22" s="15">
         <v>15</v>
       </c>
@@ -2468,7 +2467,7 @@
         <v>2.01E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="18.25" customHeight="1">
+    <row r="23" spans="1:13" ht="18.2" customHeight="1">
       <c r="A23" s="15">
         <v>16</v>
       </c>
@@ -2509,7 +2508,7 @@
         <v>2.69E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="18.25" customHeight="1">
+    <row r="24" spans="1:13" ht="18.2" customHeight="1">
       <c r="A24" s="20">
         <v>17</v>
       </c>
@@ -2550,7 +2549,7 @@
         <v>4.8099999999999997E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="18.25" customHeight="1">
+    <row r="25" spans="1:13" ht="18.2" customHeight="1">
       <c r="A25" s="20">
         <v>18</v>
       </c>
@@ -2591,7 +2590,7 @@
         <v>3.1399999999999997E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="18.25" customHeight="1">
+    <row r="26" spans="1:13" ht="18.2" customHeight="1">
       <c r="A26" s="20">
         <v>19</v>
       </c>
@@ -2632,7 +2631,7 @@
         <v>3.85E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="18.25" customHeight="1">
+    <row r="27" spans="1:13" ht="18.2" customHeight="1">
       <c r="A27" s="20">
         <v>20</v>
       </c>
@@ -2673,7 +2672,7 @@
         <v>3.7900000000000003E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="18.25" customHeight="1">
+    <row r="28" spans="1:13" ht="18.2" customHeight="1">
       <c r="A28" s="20">
         <v>21</v>
       </c>
@@ -2714,7 +2713,7 @@
         <v>3.39E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="18.25" customHeight="1">
+    <row r="29" spans="1:13" ht="18.2" customHeight="1">
       <c r="A29" s="15">
         <v>22</v>
       </c>
@@ -2755,7 +2754,7 @@
         <v>3.1199999999999999E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="18.25" customHeight="1">
+    <row r="30" spans="1:13" ht="18.2" customHeight="1">
       <c r="A30" s="15">
         <v>23</v>
       </c>
@@ -2796,7 +2795,7 @@
         <v>3.2899999999999999E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="18.25" customHeight="1">
+    <row r="31" spans="1:13" ht="18.2" customHeight="1">
       <c r="A31" s="20">
         <v>24</v>
       </c>
@@ -2837,7 +2836,7 @@
         <v>3.7499999999999999E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="18.25" customHeight="1">
+    <row r="32" spans="1:13" ht="18.2" customHeight="1">
       <c r="A32" s="20">
         <v>25</v>
       </c>
@@ -2878,7 +2877,7 @@
         <v>2.7900000000000001E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="18.25" customHeight="1">
+    <row r="33" spans="1:13" ht="18.2" customHeight="1">
       <c r="A33" s="20">
         <v>26</v>
       </c>
@@ -2919,7 +2918,7 @@
         <v>3.2800000000000003E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="18.25" customHeight="1">
+    <row r="34" spans="1:13" ht="18.2" customHeight="1">
       <c r="A34" s="20">
         <v>27</v>
       </c>
@@ -2960,7 +2959,7 @@
         <v>3.6400000000000002E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="18.25" customHeight="1">
+    <row r="35" spans="1:13" ht="18.2" customHeight="1">
       <c r="A35" s="20">
         <v>28</v>
       </c>
@@ -3001,7 +3000,7 @@
         <v>3.1199999999999999E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="18.25" customHeight="1">
+    <row r="36" spans="1:13" ht="18.2" customHeight="1">
       <c r="A36" s="15">
         <v>29</v>
       </c>
@@ -3042,7 +3041,7 @@
         <v>2.7900000000000001E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="20" customHeight="1">
+    <row r="37" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A37" s="13"/>
       <c r="B37" s="11"/>
       <c r="C37" s="12"/>
@@ -3076,7 +3075,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -3089,10 +3088,10 @@
       <selection pane="bottomRight" activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.28515625" defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
-    <col min="1" max="14" width="16.33203125" style="25" customWidth="1"/>
-    <col min="15" max="16384" width="16.33203125" style="25"/>
+    <col min="1" max="14" width="16.28515625" style="25" customWidth="1"/>
+    <col min="15" max="16384" width="16.28515625" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="27.75" customHeight="1">
@@ -3127,7 +3126,7 @@
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
     </row>
-    <row r="3" spans="1:13" ht="59.5" customHeight="1">
+    <row r="3" spans="1:13" ht="59.45" customHeight="1">
       <c r="A3" s="26" t="s">
         <v>15</v>
       </c>
@@ -3144,7 +3143,7 @@
       <c r="L3" s="9"/>
       <c r="M3" s="9"/>
     </row>
-    <row r="4" spans="1:13" ht="20" customHeight="1">
+    <row r="4" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A4" s="13"/>
       <c r="B4" s="11"/>
       <c r="C4" s="12"/>
@@ -3159,7 +3158,7 @@
       <c r="L4" s="12"/>
       <c r="M4" s="12"/>
     </row>
-    <row r="5" spans="1:13" ht="18.25" customHeight="1">
+    <row r="5" spans="1:13" ht="18.2" customHeight="1">
       <c r="A5" s="14" t="s">
         <v>7</v>
       </c>
@@ -3188,7 +3187,7 @@
       </c>
       <c r="M5" s="33"/>
     </row>
-    <row r="6" spans="1:13" ht="20" customHeight="1">
+    <row r="6" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A6" s="13"/>
       <c r="B6" s="11"/>
       <c r="C6" s="12"/>
@@ -3203,7 +3202,7 @@
       <c r="L6" s="12"/>
       <c r="M6" s="12"/>
     </row>
-    <row r="7" spans="1:13" ht="18.25" customHeight="1">
+    <row r="7" spans="1:13" ht="18.2" customHeight="1">
       <c r="A7" s="20">
         <v>1</v>
       </c>
@@ -3244,7 +3243,7 @@
         <v>1.8200000000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="18.25" customHeight="1">
+    <row r="8" spans="1:13" ht="18.2" customHeight="1">
       <c r="A8" s="20">
         <v>2</v>
       </c>
@@ -3285,7 +3284,7 @@
         <v>2.1299999999999999E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="18.25" customHeight="1">
+    <row r="9" spans="1:13" ht="18.2" customHeight="1">
       <c r="A9" s="20">
         <v>3</v>
       </c>
@@ -3326,7 +3325,7 @@
         <v>2.98E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="18.25" customHeight="1">
+    <row r="10" spans="1:13" ht="18.2" customHeight="1">
       <c r="A10" s="15">
         <v>4</v>
       </c>
@@ -3367,7 +3366,7 @@
         <v>2.3699999999999999E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="18.25" customHeight="1">
+    <row r="11" spans="1:13" ht="18.2" customHeight="1">
       <c r="A11" s="15">
         <v>5</v>
       </c>
@@ -3408,7 +3407,7 @@
         <v>2.3699999999999999E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="18.25" customHeight="1">
+    <row r="12" spans="1:13" ht="18.2" customHeight="1">
       <c r="A12" s="20">
         <v>6</v>
       </c>
@@ -3449,7 +3448,7 @@
         <v>3.5499999999999997E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="18.25" customHeight="1">
+    <row r="13" spans="1:13" ht="18.2" customHeight="1">
       <c r="A13" s="20">
         <v>7</v>
       </c>
@@ -3490,7 +3489,7 @@
         <v>4.4699999999999997E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="18.25" customHeight="1">
+    <row r="14" spans="1:13" ht="18.2" customHeight="1">
       <c r="A14" s="20">
         <v>8</v>
       </c>
@@ -3531,7 +3530,7 @@
         <v>4.6199999999999998E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="18.25" customHeight="1">
+    <row r="15" spans="1:13" ht="18.2" customHeight="1">
       <c r="A15" s="20">
         <v>9</v>
       </c>
@@ -3572,7 +3571,7 @@
         <v>3.8100000000000002E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="18.25" customHeight="1">
+    <row r="16" spans="1:13" ht="18.2" customHeight="1">
       <c r="A16" s="20">
         <v>10</v>
       </c>
@@ -3613,7 +3612,7 @@
         <v>2.9499999999999998E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="18.25" customHeight="1">
+    <row r="17" spans="1:13" ht="18.2" customHeight="1">
       <c r="A17" s="15">
         <v>11</v>
       </c>
@@ -3654,7 +3653,7 @@
         <v>2.86E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="18.25" customHeight="1">
+    <row r="18" spans="1:13" ht="18.2" customHeight="1">
       <c r="A18" s="15">
         <v>12</v>
       </c>
@@ -3695,7 +3694,7 @@
         <v>2.87E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="18.25" customHeight="1">
+    <row r="19" spans="1:13" ht="18.2" customHeight="1">
       <c r="A19" s="20">
         <v>13</v>
       </c>
@@ -3736,7 +3735,7 @@
         <v>3.6900000000000002E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="18.25" customHeight="1">
+    <row r="20" spans="1:13" ht="18.2" customHeight="1">
       <c r="A20" s="20">
         <v>14</v>
       </c>
@@ -3777,7 +3776,7 @@
         <v>3.9600000000000003E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="18.25" customHeight="1">
+    <row r="21" spans="1:13" ht="18.2" customHeight="1">
       <c r="A21" s="20">
         <v>15</v>
       </c>
@@ -3818,7 +3817,7 @@
         <v>3.8899999999999997E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="18.25" customHeight="1">
+    <row r="22" spans="1:13" ht="18.2" customHeight="1">
       <c r="A22" s="20">
         <v>16</v>
       </c>
@@ -3859,7 +3858,7 @@
         <v>3.1300000000000001E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="18.25" customHeight="1">
+    <row r="23" spans="1:13" ht="18.2" customHeight="1">
       <c r="A23" s="20">
         <v>17</v>
       </c>
@@ -3900,7 +3899,7 @@
         <v>2.6200000000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="18.25" customHeight="1">
+    <row r="24" spans="1:13" ht="18.2" customHeight="1">
       <c r="A24" s="15">
         <v>18</v>
       </c>
@@ -3941,7 +3940,7 @@
         <v>1.9E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="18.25" customHeight="1">
+    <row r="25" spans="1:13" ht="18.2" customHeight="1">
       <c r="A25" s="15">
         <v>19</v>
       </c>
@@ -3982,7 +3981,7 @@
         <v>2.6499999999999999E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="18.25" customHeight="1">
+    <row r="26" spans="1:13" ht="18.2" customHeight="1">
       <c r="A26" s="20">
         <v>20</v>
       </c>
@@ -4023,7 +4022,7 @@
         <v>3.6200000000000003E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="18.25" customHeight="1">
+    <row r="27" spans="1:13" ht="18.2" customHeight="1">
       <c r="A27" s="20">
         <v>21</v>
       </c>
@@ -4064,7 +4063,7 @@
         <v>2.81E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="18.25" customHeight="1">
+    <row r="28" spans="1:13" ht="18.2" customHeight="1">
       <c r="A28" s="20">
         <v>22</v>
       </c>
@@ -4105,7 +4104,7 @@
         <v>4.1500000000000002E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="18.25" customHeight="1">
+    <row r="29" spans="1:13" ht="18.2" customHeight="1">
       <c r="A29" s="20">
         <v>23</v>
       </c>
@@ -4146,7 +4145,7 @@
         <v>3.5499999999999997E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="18.25" customHeight="1">
+    <row r="30" spans="1:13" ht="18.2" customHeight="1">
       <c r="A30" s="20">
         <v>24</v>
       </c>
@@ -4187,7 +4186,7 @@
         <v>3.9100000000000003E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="18.25" customHeight="1">
+    <row r="31" spans="1:13" ht="18.2" customHeight="1">
       <c r="A31" s="15">
         <v>25</v>
       </c>
@@ -4228,7 +4227,7 @@
         <v>2.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="18.25" customHeight="1">
+    <row r="32" spans="1:13" ht="18.2" customHeight="1">
       <c r="A32" s="15">
         <v>26</v>
       </c>
@@ -4269,7 +4268,7 @@
         <v>2.98E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="18.25" customHeight="1">
+    <row r="33" spans="1:13" ht="18.2" customHeight="1">
       <c r="A33" s="20">
         <v>27</v>
       </c>
@@ -4310,7 +4309,7 @@
         <v>3.49E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="18.25" customHeight="1">
+    <row r="34" spans="1:13" ht="18.2" customHeight="1">
       <c r="A34" s="20">
         <v>28</v>
       </c>
@@ -4351,7 +4350,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="18.25" customHeight="1">
+    <row r="35" spans="1:13" ht="18.2" customHeight="1">
       <c r="A35" s="20">
         <v>29</v>
       </c>
@@ -4392,7 +4391,7 @@
         <v>5.11E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="18.25" customHeight="1">
+    <row r="36" spans="1:13" ht="18.2" customHeight="1">
       <c r="A36" s="20">
         <v>30</v>
       </c>
@@ -4433,7 +4432,7 @@
         <v>3.2800000000000003E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="18.25" customHeight="1">
+    <row r="37" spans="1:13" ht="18.2" customHeight="1">
       <c r="A37" s="20">
         <v>31</v>
       </c>
@@ -4474,7 +4473,7 @@
         <v>2.63E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="20" customHeight="1">
+    <row r="38" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A38" s="13"/>
       <c r="B38" s="11"/>
       <c r="C38" s="12"/>
@@ -4508,7 +4507,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -4521,10 +4520,10 @@
       <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.28515625" defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
-    <col min="1" max="14" width="16.33203125" style="27" customWidth="1"/>
-    <col min="15" max="16384" width="16.33203125" style="27"/>
+    <col min="1" max="14" width="16.28515625" style="27" customWidth="1"/>
+    <col min="15" max="16384" width="16.28515625" style="27"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="27.75" customHeight="1">
@@ -4559,7 +4558,7 @@
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
     </row>
-    <row r="3" spans="1:13" ht="59.5" customHeight="1">
+    <row r="3" spans="1:13" ht="59.45" customHeight="1">
       <c r="A3" s="26" t="s">
         <v>17</v>
       </c>
@@ -4576,7 +4575,7 @@
       <c r="L3" s="9"/>
       <c r="M3" s="9"/>
     </row>
-    <row r="4" spans="1:13" ht="20" customHeight="1">
+    <row r="4" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A4" s="13"/>
       <c r="B4" s="11"/>
       <c r="C4" s="12"/>
@@ -4591,7 +4590,7 @@
       <c r="L4" s="12"/>
       <c r="M4" s="12"/>
     </row>
-    <row r="5" spans="1:13" ht="18.25" customHeight="1">
+    <row r="5" spans="1:13" ht="18.2" customHeight="1">
       <c r="A5" s="14" t="s">
         <v>7</v>
       </c>
@@ -4620,7 +4619,7 @@
       </c>
       <c r="M5" s="33"/>
     </row>
-    <row r="6" spans="1:13" ht="20" customHeight="1">
+    <row r="6" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A6" s="13"/>
       <c r="B6" s="11"/>
       <c r="C6" s="12"/>
@@ -4635,7 +4634,7 @@
       <c r="L6" s="12"/>
       <c r="M6" s="12"/>
     </row>
-    <row r="7" spans="1:13" ht="18.25" customHeight="1">
+    <row r="7" spans="1:13" ht="18.2" customHeight="1">
       <c r="A7" s="15">
         <v>1</v>
       </c>
@@ -4676,7 +4675,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="18.25" customHeight="1">
+    <row r="8" spans="1:13" ht="18.2" customHeight="1">
       <c r="A8" s="20">
         <v>2</v>
       </c>
@@ -4717,7 +4716,7 @@
         <v>1.54E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="18.25" customHeight="1">
+    <row r="9" spans="1:13" ht="18.2" customHeight="1">
       <c r="A9" s="20">
         <v>3</v>
       </c>
@@ -4758,7 +4757,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="18.25" customHeight="1">
+    <row r="10" spans="1:13" ht="18.2" customHeight="1">
       <c r="A10" s="20">
         <v>4</v>
       </c>
@@ -4799,7 +4798,7 @@
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="18.25" customHeight="1">
+    <row r="11" spans="1:13" ht="18.2" customHeight="1">
       <c r="A11" s="20">
         <v>5</v>
       </c>
@@ -4840,7 +4839,7 @@
         <v>1.2699999999999999E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="18.25" customHeight="1">
+    <row r="12" spans="1:13" ht="18.2" customHeight="1">
       <c r="A12" s="20">
         <v>6</v>
       </c>
@@ -4881,7 +4880,7 @@
         <v>1.06E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="18.25" customHeight="1">
+    <row r="13" spans="1:13" ht="18.2" customHeight="1">
       <c r="A13" s="15">
         <v>7</v>
       </c>
@@ -4922,7 +4921,7 @@
         <v>7.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="18.25" customHeight="1">
+    <row r="14" spans="1:13" ht="18.2" customHeight="1">
       <c r="A14" s="15">
         <v>8</v>
       </c>
@@ -4963,7 +4962,7 @@
         <v>1.21E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="18.25" customHeight="1">
+    <row r="15" spans="1:13" ht="18.2" customHeight="1">
       <c r="A15" s="20">
         <v>9</v>
       </c>
@@ -5004,7 +5003,7 @@
         <v>1.24E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="18.25" customHeight="1">
+    <row r="16" spans="1:13" ht="18.2" customHeight="1">
       <c r="A16" s="20">
         <v>10</v>
       </c>
@@ -5045,7 +5044,7 @@
         <v>1.61E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="18.25" customHeight="1">
+    <row r="17" spans="1:13" ht="18.2" customHeight="1">
       <c r="A17" s="20">
         <v>11</v>
       </c>
@@ -5086,7 +5085,7 @@
         <v>1.3899999999999999E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="18.25" customHeight="1">
+    <row r="18" spans="1:13" ht="18.2" customHeight="1">
       <c r="A18" s="20">
         <v>12</v>
       </c>
@@ -5127,7 +5126,7 @@
         <v>1.6899999999999998E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="18.25" customHeight="1">
+    <row r="19" spans="1:13" ht="18.2" customHeight="1">
       <c r="A19" s="20">
         <v>13</v>
       </c>
@@ -5168,7 +5167,7 @@
         <v>7.2599999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="18.25" customHeight="1">
+    <row r="20" spans="1:13" ht="18.2" customHeight="1">
       <c r="A20" s="15">
         <v>14</v>
       </c>
@@ -5209,7 +5208,7 @@
         <v>6.3100000000000003E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="18.25" customHeight="1">
+    <row r="21" spans="1:13" ht="18.2" customHeight="1">
       <c r="A21" s="15">
         <v>15</v>
       </c>
@@ -5250,7 +5249,7 @@
         <v>6.6400000000000001E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="18.25" customHeight="1">
+    <row r="22" spans="1:13" ht="18.2" customHeight="1">
       <c r="A22" s="20">
         <v>16</v>
       </c>
@@ -5291,7 +5290,7 @@
         <v>7.1900000000000006E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="18.25" customHeight="1">
+    <row r="23" spans="1:13" ht="18.2" customHeight="1">
       <c r="A23" s="20">
         <v>17</v>
       </c>
@@ -5332,7 +5331,7 @@
         <v>5.57E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="18.25" customHeight="1">
+    <row r="24" spans="1:13" ht="18.2" customHeight="1">
       <c r="A24" s="20">
         <v>18</v>
       </c>
@@ -5373,7 +5372,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="18.25" customHeight="1">
+    <row r="25" spans="1:13" ht="18.2" customHeight="1">
       <c r="A25" s="20">
         <v>19</v>
       </c>
@@ -5414,7 +5413,7 @@
         <v>6.3500000000000001E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="18.25" customHeight="1">
+    <row r="26" spans="1:13" ht="18.2" customHeight="1">
       <c r="A26" s="20">
         <v>20</v>
       </c>
@@ -5455,7 +5454,7 @@
         <v>3.27E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="18.25" customHeight="1">
+    <row r="27" spans="1:13" ht="18.2" customHeight="1">
       <c r="A27" s="15">
         <v>21</v>
       </c>
@@ -5496,7 +5495,7 @@
         <v>2.87E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="18.25" customHeight="1">
+    <row r="28" spans="1:13" ht="18.2" customHeight="1">
       <c r="A28" s="15">
         <v>22</v>
       </c>
@@ -5537,7 +5536,7 @@
         <v>2.5600000000000001E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="18.25" customHeight="1">
+    <row r="29" spans="1:13" ht="18.2" customHeight="1">
       <c r="A29" s="20">
         <v>23</v>
       </c>
@@ -5578,7 +5577,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="18.25" customHeight="1">
+    <row r="30" spans="1:13" ht="18.2" customHeight="1">
       <c r="A30" s="20">
         <v>24</v>
       </c>
@@ -5619,7 +5618,7 @@
         <v>3.32E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="18.25" customHeight="1">
+    <row r="31" spans="1:13" ht="18.2" customHeight="1">
       <c r="A31" s="20">
         <v>25</v>
       </c>
@@ -5660,7 +5659,7 @@
         <v>3.7699999999999997E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="18.25" customHeight="1">
+    <row r="32" spans="1:13" ht="18.2" customHeight="1">
       <c r="A32" s="20">
         <v>26</v>
       </c>
@@ -5701,7 +5700,7 @@
         <v>3.5200000000000002E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="18.25" customHeight="1">
+    <row r="33" spans="1:13" ht="18.2" customHeight="1">
       <c r="A33" s="20">
         <v>27</v>
       </c>
@@ -5742,7 +5741,7 @@
         <v>2.98E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="18.25" customHeight="1">
+    <row r="34" spans="1:13" ht="18.2" customHeight="1">
       <c r="A34" s="15">
         <v>28</v>
       </c>
@@ -5783,7 +5782,7 @@
         <v>1.47E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="18.25" customHeight="1">
+    <row r="35" spans="1:13" ht="18.2" customHeight="1">
       <c r="A35" s="15">
         <v>29</v>
       </c>
@@ -5824,7 +5823,7 @@
         <v>1.8700000000000001E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="18.25" customHeight="1">
+    <row r="36" spans="1:13" ht="18.2" customHeight="1">
       <c r="A36" s="20">
         <v>30</v>
       </c>
@@ -5865,7 +5864,7 @@
         <v>4.2999999999999997E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="18.25" customHeight="1">
+    <row r="37" spans="1:13" ht="18.2" customHeight="1">
       <c r="A37" s="20">
         <v>31</v>
       </c>
@@ -5906,7 +5905,7 @@
         <v>6.08E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="20" customHeight="1">
+    <row r="38" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A38" s="13"/>
       <c r="B38" s="11"/>
       <c r="C38" s="12"/>
@@ -5940,7 +5939,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -5950,13 +5949,13 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="B5" sqref="B5:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.28515625" defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
-    <col min="1" max="14" width="16.33203125" style="28" customWidth="1"/>
-    <col min="15" max="16384" width="16.33203125" style="28"/>
+    <col min="1" max="14" width="16.28515625" style="28" customWidth="1"/>
+    <col min="15" max="16384" width="16.28515625" style="28"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="27.75" customHeight="1">
@@ -5991,7 +5990,7 @@
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
     </row>
-    <row r="3" spans="1:13" ht="59.5" customHeight="1">
+    <row r="3" spans="1:13" ht="59.45" customHeight="1">
       <c r="A3" s="26" t="s">
         <v>19</v>
       </c>
@@ -6008,7 +6007,7 @@
       <c r="L3" s="9"/>
       <c r="M3" s="9"/>
     </row>
-    <row r="4" spans="1:13" ht="20" customHeight="1">
+    <row r="4" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A4" s="13"/>
       <c r="B4" s="11"/>
       <c r="C4" s="12"/>
@@ -6023,7 +6022,7 @@
       <c r="L4" s="12"/>
       <c r="M4" s="12"/>
     </row>
-    <row r="5" spans="1:13" ht="18.25" customHeight="1">
+    <row r="5" spans="1:13" ht="18.2" customHeight="1">
       <c r="A5" s="14" t="s">
         <v>7</v>
       </c>
@@ -6052,7 +6051,7 @@
       </c>
       <c r="M5" s="33"/>
     </row>
-    <row r="6" spans="1:13" ht="20" customHeight="1">
+    <row r="6" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A6" s="13"/>
       <c r="B6" s="11"/>
       <c r="C6" s="12"/>
@@ -6067,7 +6066,7 @@
       <c r="L6" s="12"/>
       <c r="M6" s="12"/>
     </row>
-    <row r="7" spans="1:13" ht="18.25" customHeight="1">
+    <row r="7" spans="1:13" ht="18.2" customHeight="1">
       <c r="A7" s="20">
         <v>1</v>
       </c>
@@ -6108,7 +6107,7 @@
         <v>8.1799999999999998E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="18.25" customHeight="1">
+    <row r="8" spans="1:13" ht="18.2" customHeight="1">
       <c r="A8" s="20">
         <v>2</v>
       </c>
@@ -6149,7 +6148,7 @@
         <v>6.6600000000000006E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="18.25" customHeight="1">
+    <row r="9" spans="1:13" ht="18.2" customHeight="1">
       <c r="A9" s="20">
         <v>3</v>
       </c>
@@ -6190,7 +6189,7 @@
         <v>4.0599999999999997E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="18.25" customHeight="1">
+    <row r="10" spans="1:13" ht="18.2" customHeight="1">
       <c r="A10" s="15">
         <v>4</v>
       </c>
@@ -6231,7 +6230,7 @@
         <v>2.3400000000000001E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="18.25" customHeight="1">
+    <row r="11" spans="1:13" ht="18.2" customHeight="1">
       <c r="A11" s="15">
         <v>5</v>
       </c>
@@ -6272,7 +6271,7 @@
         <v>2.3900000000000001E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="18.25" customHeight="1">
+    <row r="12" spans="1:13" ht="18.2" customHeight="1">
       <c r="A12" s="20">
         <v>6</v>
       </c>
@@ -6313,7 +6312,7 @@
         <v>4.5400000000000003E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="18.25" customHeight="1">
+    <row r="13" spans="1:13" ht="18.2" customHeight="1">
       <c r="A13" s="20">
         <v>7</v>
       </c>
@@ -6354,7 +6353,7 @@
         <v>4.0500000000000001E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="18.25" customHeight="1">
+    <row r="14" spans="1:13" ht="18.2" customHeight="1">
       <c r="A14" s="20">
         <v>8</v>
       </c>
@@ -6395,7 +6394,7 @@
         <v>3.3500000000000002E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="18.25" customHeight="1">
+    <row r="15" spans="1:13" ht="18.2" customHeight="1">
       <c r="A15" s="20">
         <v>9</v>
       </c>
@@ -6436,7 +6435,7 @@
         <v>3.04E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="18.25" customHeight="1">
+    <row r="16" spans="1:13" ht="18.2" customHeight="1">
       <c r="A16" s="20">
         <v>10</v>
       </c>
@@ -6477,7 +6476,7 @@
         <v>1.8599999999999998E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="18.25" customHeight="1">
+    <row r="17" spans="1:13" ht="18.2" customHeight="1">
       <c r="A17" s="15">
         <v>11</v>
       </c>
@@ -6518,7 +6517,7 @@
         <v>1.47E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="18.25" customHeight="1">
+    <row r="18" spans="1:13" ht="18.2" customHeight="1">
       <c r="A18" s="15">
         <v>12</v>
       </c>
@@ -6559,7 +6558,7 @@
         <v>1.5299999999999999E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="18.25" customHeight="1">
+    <row r="19" spans="1:13" ht="18.2" customHeight="1">
       <c r="A19" s="20">
         <v>13</v>
       </c>
@@ -6600,7 +6599,7 @@
         <v>1.8700000000000001E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="18.25" customHeight="1">
+    <row r="20" spans="1:13" ht="18.2" customHeight="1">
       <c r="A20" s="20">
         <v>14</v>
       </c>
@@ -6641,7 +6640,7 @@
         <v>4.7699999999999999E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="18.25" customHeight="1">
+    <row r="21" spans="1:13" ht="18.2" customHeight="1">
       <c r="A21" s="20">
         <v>15</v>
       </c>
@@ -6682,7 +6681,7 @@
         <v>2.8199999999999999E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="18.25" customHeight="1">
+    <row r="22" spans="1:13" ht="18.2" customHeight="1">
       <c r="A22" s="20">
         <v>16</v>
       </c>
@@ -6723,7 +6722,7 @@
         <v>3.3599999999999998E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="18.25" customHeight="1">
+    <row r="23" spans="1:13" ht="18.2" customHeight="1">
       <c r="A23" s="20">
         <v>17</v>
       </c>
@@ -6764,7 +6763,7 @@
         <v>3.0300000000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="18.25" customHeight="1">
+    <row r="24" spans="1:13" ht="18.2" customHeight="1">
       <c r="A24" s="15">
         <v>18</v>
       </c>
@@ -6805,7 +6804,7 @@
         <v>1.7299999999999999E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="18.25" customHeight="1">
+    <row r="25" spans="1:13" ht="18.2" customHeight="1">
       <c r="A25" s="15">
         <v>19</v>
       </c>
@@ -6846,7 +6845,7 @@
         <v>1.77E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="18.25" customHeight="1">
+    <row r="26" spans="1:13" ht="18.2" customHeight="1">
       <c r="A26" s="20">
         <v>20</v>
       </c>
@@ -6887,7 +6886,7 @@
         <v>3.73E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="18.25" customHeight="1">
+    <row r="27" spans="1:13" ht="18.2" customHeight="1">
       <c r="A27" s="20">
         <v>21</v>
       </c>
@@ -6928,7 +6927,7 @@
         <v>3.2599999999999997E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="18.25" customHeight="1">
+    <row r="28" spans="1:13" ht="18.2" customHeight="1">
       <c r="A28" s="20">
         <v>22</v>
       </c>
@@ -6969,7 +6968,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="18.25" customHeight="1">
+    <row r="29" spans="1:13" ht="18.2" customHeight="1">
       <c r="A29" s="20">
         <v>23</v>
       </c>
@@ -7010,7 +7009,7 @@
         <v>3.1E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="18.25" customHeight="1">
+    <row r="30" spans="1:13" ht="18.2" customHeight="1">
       <c r="A30" s="20">
         <v>24</v>
       </c>
@@ -7051,7 +7050,7 @@
         <v>2.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="18.25" customHeight="1">
+    <row r="31" spans="1:13" ht="18.2" customHeight="1">
       <c r="A31" s="15">
         <v>25</v>
       </c>
@@ -7092,7 +7091,7 @@
         <v>2.52E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="18.25" customHeight="1">
+    <row r="32" spans="1:13" ht="18.2" customHeight="1">
       <c r="A32" s="15">
         <v>26</v>
       </c>
@@ -7133,7 +7132,7 @@
         <v>2.0500000000000001E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="18.25" customHeight="1">
+    <row r="33" spans="1:13" ht="18.2" customHeight="1">
       <c r="A33" s="20">
         <v>27</v>
       </c>
@@ -7174,7 +7173,7 @@
         <v>2.9600000000000001E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="18.25" customHeight="1">
+    <row r="34" spans="1:13" ht="18.2" customHeight="1">
       <c r="A34" s="20">
         <v>28</v>
       </c>
@@ -7215,7 +7214,7 @@
         <v>2.7400000000000001E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="18.25" customHeight="1">
+    <row r="35" spans="1:13" ht="18.2" customHeight="1">
       <c r="A35" s="20">
         <v>29</v>
       </c>
@@ -7256,7 +7255,7 @@
         <v>6.8699999999999997E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="18.25" customHeight="1">
+    <row r="36" spans="1:13" ht="18.2" customHeight="1">
       <c r="A36" s="20">
         <v>30</v>
       </c>

</xml_diff>